<commit_message>
the plane is successfully following share price data
</commit_message>
<xml_diff>
--- a/data/airbus.xlsx
+++ b/data/airbus.xlsx
@@ -3301,11 +3301,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="680867624"/>
-        <c:axId val="680870712"/>
+        <c:axId val="748203192"/>
+        <c:axId val="748206232"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="680867624"/>
+        <c:axId val="748203192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3315,14 +3315,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="680870712"/>
+        <c:crossAx val="748206232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="680870712"/>
+        <c:axId val="748206232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3332,14 +3332,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="680867624"/>
+        <c:crossAx val="748203192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16916,15 +16915,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -16938,7 +16937,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>36738</v>
       </c>
@@ -16946,7 +16945,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>36769</v>
       </c>
@@ -16954,7 +16953,7 @@
         <v>17.940000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>36798</v>
       </c>
@@ -16962,7 +16961,7 @@
         <v>19.850000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>36830</v>
       </c>
@@ -16970,7 +16969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>36860</v>
       </c>
@@ -16978,7 +16977,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>36889</v>
       </c>
@@ -16986,7 +16985,7 @@
         <v>23.66</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>36922</v>
       </c>
@@ -16994,7 +16993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>36950</v>
       </c>
@@ -17002,11 +17001,11 @@
         <v>22.5</v>
       </c>
       <c r="C9">
-        <f>AVERAGE(B2:B16)</f>
+        <f t="shared" ref="C9:C40" si="0">AVERAGE(B2:B16)</f>
         <v>20.866666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>36980</v>
       </c>
@@ -17014,15 +17013,19 @@
         <v>21.01</v>
       </c>
       <c r="C10">
-        <f>AVERAGE(B3:B17)</f>
+        <f t="shared" si="0"/>
         <v>20.52</v>
       </c>
       <c r="D10">
-        <f>(C11-C9)/(A11-A9)</f>
+        <f t="shared" ref="D10:D41" si="1">(C11-C9)/(A11-A9)</f>
         <v>-1.0710382513661246E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <f>C10-C9</f>
+        <v>-0.34666666666666757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>37011</v>
       </c>
@@ -17030,15 +17033,19 @@
         <v>20.5</v>
       </c>
       <c r="C11">
-        <f>AVERAGE(B4:B18)</f>
+        <f t="shared" si="0"/>
         <v>20.213333333333331</v>
       </c>
       <c r="D11">
-        <f>(C12-C10)/(A12-A10)</f>
+        <f t="shared" si="1"/>
         <v>-1.1623655913978547E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <f t="shared" ref="E11:E74" si="2">C11-C10</f>
+        <v>-0.30666666666666842</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>37042</v>
       </c>
@@ -17046,15 +17053,19 @@
         <v>23.22</v>
       </c>
       <c r="C12">
-        <f>AVERAGE(B5:B19)</f>
+        <f t="shared" si="0"/>
         <v>19.79933333333333</v>
       </c>
       <c r="D12">
-        <f>(C13-C11)/(A13-A11)</f>
+        <f t="shared" si="1"/>
         <v>-1.9122222222222263E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>-0.41400000000000148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>37071</v>
       </c>
@@ -17062,15 +17073,19 @@
         <v>21.75</v>
       </c>
       <c r="C13">
-        <f>AVERAGE(B6:B20)</f>
+        <f t="shared" si="0"/>
         <v>19.065999999999995</v>
       </c>
       <c r="D13">
-        <f>(C14-C12)/(A14-A12)</f>
+        <f t="shared" si="1"/>
         <v>-2.2437158469945345E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>-0.73333333333333428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>37103</v>
       </c>
@@ -17078,15 +17093,19 @@
         <v>22.7</v>
       </c>
       <c r="C14">
-        <f>AVERAGE(B7:B21)</f>
+        <f t="shared" si="0"/>
         <v>18.430666666666664</v>
       </c>
       <c r="D14">
-        <f>(C15-C13)/(A15-A13)</f>
+        <f t="shared" si="1"/>
         <v>-1.8021164021163882E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>-0.63533333333333175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>37134</v>
       </c>
@@ -17094,15 +17113,19 @@
         <v>18.82</v>
       </c>
       <c r="C15">
-        <f>AVERAGE(B8:B22)</f>
+        <f t="shared" si="0"/>
         <v>17.930666666666671</v>
       </c>
       <c r="D15">
-        <f>(C16-C14)/(A16-A14)</f>
+        <f t="shared" si="1"/>
         <v>-1.5683615819208997E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>-0.49999999999999289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>37162</v>
       </c>
@@ -17110,15 +17133,19 @@
         <v>11.85</v>
       </c>
       <c r="C16">
-        <f>AVERAGE(B9:B23)</f>
+        <f t="shared" si="0"/>
         <v>17.505333333333333</v>
       </c>
       <c r="D16">
-        <f>(C17-C15)/(A17-A15)</f>
+        <f t="shared" si="1"/>
         <v>-1.2557377049180357E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>-0.425333333333338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>37195</v>
       </c>
@@ -17126,15 +17153,19 @@
         <v>12.9</v>
       </c>
       <c r="C17">
-        <f>AVERAGE(B10:B24)</f>
+        <f t="shared" si="0"/>
         <v>17.164666666666669</v>
       </c>
       <c r="D17">
-        <f>(C18-C16)/(A18-A16)</f>
+        <f t="shared" si="1"/>
         <v>-1.1164021164021105E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>-0.34066666666666379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>37225</v>
       </c>
@@ -17142,15 +17173,19 @@
         <v>13.34</v>
       </c>
       <c r="C18">
-        <f>AVERAGE(B11:B25)</f>
+        <f t="shared" si="0"/>
         <v>16.802000000000003</v>
       </c>
       <c r="D18">
-        <f>(C19-C17)/(A19-A17)</f>
+        <f t="shared" si="1"/>
         <v>-1.0808743169398897E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>-0.3626666666666658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>37256</v>
       </c>
@@ -17158,15 +17193,19 @@
         <v>13.64</v>
       </c>
       <c r="C19">
-        <f>AVERAGE(B12:B26)</f>
+        <f t="shared" si="0"/>
         <v>16.505333333333336</v>
       </c>
       <c r="D19">
-        <f>(C20-C18)/(A20-A18)</f>
+        <f t="shared" si="1"/>
         <v>-1.5096774193548415E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>-0.29666666666666686</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>37287</v>
       </c>
@@ -17174,15 +17213,19 @@
         <v>13</v>
       </c>
       <c r="C20">
-        <f>AVERAGE(B13:B27)</f>
+        <f t="shared" si="0"/>
         <v>15.866000000000001</v>
       </c>
       <c r="D20">
-        <f>(C21-C19)/(A21-A19)</f>
+        <f t="shared" si="1"/>
         <v>-2.3265536723163883E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>-0.63933333333333486</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>37315</v>
       </c>
@@ -17190,15 +17233,19 @@
         <v>14.57</v>
       </c>
       <c r="C21">
-        <f>AVERAGE(B14:B28)</f>
+        <f t="shared" si="0"/>
         <v>15.132666666666667</v>
       </c>
       <c r="D21">
-        <f>(C22-C20)/(A22-A20)</f>
+        <f t="shared" si="1"/>
         <v>-2.6362573099415199E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>-0.73333333333333428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>37344</v>
       </c>
@@ -17206,15 +17253,19 @@
         <v>16.16</v>
       </c>
       <c r="C22">
-        <f>AVERAGE(B15:B29)</f>
+        <f t="shared" si="0"/>
         <v>14.363333333333335</v>
       </c>
       <c r="D22">
-        <f>(C23-C21)/(A23-A21)</f>
+        <f t="shared" si="1"/>
         <v>-1.9202185792349724E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>-0.76933333333333209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>37376</v>
       </c>
@@ -17222,15 +17273,19 @@
         <v>16.62</v>
       </c>
       <c r="C23">
-        <f>AVERAGE(B16:B30)</f>
+        <f t="shared" si="0"/>
         <v>13.961333333333334</v>
       </c>
       <c r="D23">
-        <f>(C24-C22)/(A24-A22)</f>
+        <f t="shared" si="1"/>
         <v>-8.4973544973545347E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>-0.40200000000000102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>37407</v>
       </c>
@@ -17238,15 +17293,19 @@
         <v>17.39</v>
       </c>
       <c r="C24">
-        <f>AVERAGE(B17:B31)</f>
+        <f t="shared" si="0"/>
         <v>13.827999999999999</v>
       </c>
       <c r="D24">
-        <f>(C25-C23)/(A25-A23)</f>
+        <f t="shared" si="1"/>
         <v>-5.8757062146892807E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>-0.13333333333333464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>37435</v>
       </c>
@@ -17254,15 +17313,19 @@
         <v>15.57</v>
       </c>
       <c r="C25">
-        <f>AVERAGE(B18:B32)</f>
+        <f t="shared" si="0"/>
         <v>13.614666666666666</v>
       </c>
       <c r="D25">
-        <f>(C26-C24)/(A26-A24)</f>
+        <f t="shared" si="1"/>
         <v>-9.2568306010929104E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>-0.21333333333333293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>37468</v>
       </c>
@@ -17270,15 +17333,19 @@
         <v>16.05</v>
       </c>
       <c r="C26">
-        <f>AVERAGE(B19:B33)</f>
+        <f t="shared" si="0"/>
         <v>13.263333333333332</v>
       </c>
       <c r="D26">
-        <f>(C27-C25)/(A27-A25)</f>
+        <f t="shared" si="1"/>
         <v>-1.2708994708994734E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>-0.35133333333333461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>37498</v>
       </c>
@@ -17286,15 +17353,19 @@
         <v>13.63</v>
       </c>
       <c r="C27">
-        <f>AVERAGE(B20:B34)</f>
+        <f t="shared" si="0"/>
         <v>12.813999999999998</v>
       </c>
       <c r="D27">
-        <f>(C28-C26)/(A28-A26)</f>
+        <f t="shared" si="1"/>
         <v>-1.2469945355191237E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>-0.44933333333333358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>37529</v>
       </c>
@@ -17302,15 +17373,19 @@
         <v>10.75</v>
       </c>
       <c r="C28">
-        <f>AVERAGE(B21:B35)</f>
+        <f t="shared" si="0"/>
         <v>12.502666666666666</v>
       </c>
       <c r="D28">
-        <f>(C29-C27)/(A29-A27)</f>
+        <f t="shared" si="1"/>
         <v>-1.0505376344085996E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>-0.31133333333333191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>37560</v>
       </c>
@@ -17318,15 +17393,19 @@
         <v>11.16</v>
       </c>
       <c r="C29">
-        <f>AVERAGE(B22:B36)</f>
+        <f t="shared" si="0"/>
         <v>12.162666666666667</v>
       </c>
       <c r="D29">
-        <f>(C30-C28)/(A30-A28)</f>
+        <f t="shared" si="1"/>
         <v>-1.1755555555555535E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>-0.33999999999999986</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>37589</v>
       </c>
@@ -17334,15 +17413,19 @@
         <v>12.79</v>
       </c>
       <c r="C30">
-        <f>AVERAGE(B23:B37)</f>
+        <f t="shared" si="0"/>
         <v>11.797333333333334</v>
       </c>
       <c r="D30">
-        <f>(C31-C29)/(A31-A29)</f>
+        <f t="shared" si="1"/>
         <v>-8.6666666666666298E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>-0.36533333333333218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>37621</v>
       </c>
@@ -17350,15 +17433,19 @@
         <v>9.85</v>
       </c>
       <c r="C31">
-        <f>AVERAGE(B24:B38)</f>
+        <f t="shared" si="0"/>
         <v>11.634000000000002</v>
       </c>
       <c r="D31">
-        <f>(C32-C30)/(A32-A30)</f>
+        <f t="shared" si="1"/>
         <v>-5.7566137566137715E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>-0.16333333333333222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>37652</v>
       </c>
@@ -17366,15 +17453,19 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="C32">
-        <f>AVERAGE(B25:B39)</f>
+        <f t="shared" si="0"/>
         <v>11.434666666666667</v>
       </c>
       <c r="D32">
-        <f>(C33-C31)/(A33-A31)</f>
+        <f t="shared" si="1"/>
         <v>-6.0112994350282794E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>-0.19933333333333536</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>37680</v>
       </c>
@@ -17382,15 +17473,19 @@
         <v>8.07</v>
       </c>
       <c r="C33">
-        <f>AVERAGE(B26:B40)</f>
+        <f t="shared" si="0"/>
         <v>11.279333333333334</v>
       </c>
       <c r="D33">
-        <f>(C34-C32)/(A34-A32)</f>
+        <f t="shared" si="1"/>
         <v>-9.943502824858565E-4</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>-0.1553333333333331</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>37711</v>
       </c>
@@ -17398,15 +17493,19 @@
         <v>6.9</v>
       </c>
       <c r="C34">
-        <f>AVERAGE(B27:B41)</f>
+        <f t="shared" si="0"/>
         <v>11.376000000000001</v>
       </c>
       <c r="D34">
-        <f>(C35-C33)/(A35-A33)</f>
+        <f t="shared" si="1"/>
         <v>6.5792349726775702E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>9.6666666666667567E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>37741</v>
       </c>
@@ -17414,15 +17513,19 @@
         <v>8.33</v>
       </c>
       <c r="C35">
-        <f>AVERAGE(B28:B42)</f>
+        <f t="shared" si="0"/>
         <v>11.680666666666665</v>
       </c>
       <c r="D35">
-        <f>(C36-C34)/(A36-A34)</f>
+        <f t="shared" si="1"/>
         <v>1.4077777777777722E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>0.3046666666666642</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>37771</v>
       </c>
@@ -17430,15 +17533,19 @@
         <v>9.4700000000000006</v>
       </c>
       <c r="C36">
-        <f>AVERAGE(B29:B43)</f>
+        <f t="shared" si="0"/>
         <v>12.220666666666665</v>
       </c>
       <c r="D36">
-        <f>(C37-C35)/(A37-A35)</f>
+        <f t="shared" si="1"/>
         <v>1.5737704918032801E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>0.53999999999999915</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>37802</v>
       </c>
@@ -17446,15 +17553,19 @@
         <v>10.68</v>
       </c>
       <c r="C37">
-        <f>AVERAGE(B30:B44)</f>
+        <f t="shared" si="0"/>
         <v>12.640666666666666</v>
       </c>
       <c r="D37">
-        <f>(C38-C36)/(A38-A36)</f>
+        <f t="shared" si="1"/>
         <v>1.3032258064516184E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>0.42000000000000171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>37833</v>
       </c>
@@ -17462,15 +17573,19 @@
         <v>14.17</v>
       </c>
       <c r="C38">
-        <f>AVERAGE(B31:B45)</f>
+        <f t="shared" si="0"/>
         <v>13.028666666666668</v>
       </c>
       <c r="D38">
-        <f>(C39-C37)/(A39-A37)</f>
+        <f t="shared" si="1"/>
         <v>1.5022222222222225E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>0.38800000000000168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>37862</v>
       </c>
@@ -17478,15 +17593,19 @@
         <v>14.4</v>
       </c>
       <c r="C39">
-        <f>AVERAGE(B32:B46)</f>
+        <f t="shared" si="0"/>
         <v>13.542</v>
       </c>
       <c r="D39">
-        <f>(C40-C38)/(A40-A38)</f>
+        <f t="shared" si="1"/>
         <v>2.0874316939890683E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>0.51333333333333186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>37894</v>
       </c>
@@ -17494,15 +17613,19 @@
         <v>13.24</v>
       </c>
       <c r="C40">
-        <f>AVERAGE(B33:B47)</f>
+        <f t="shared" si="0"/>
         <v>14.302</v>
       </c>
       <c r="D40">
-        <f>(C41-C39)/(A41-A39)</f>
+        <f t="shared" si="1"/>
         <v>2.5058201058201061E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>0.75999999999999979</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>37925</v>
       </c>
@@ -17510,15 +17633,19 @@
         <v>17.5</v>
       </c>
       <c r="C41">
-        <f>AVERAGE(B34:B48)</f>
+        <f t="shared" ref="C41:C72" si="3">AVERAGE(B34:B48)</f>
         <v>15.120666666666667</v>
       </c>
       <c r="D41">
-        <f>(C42-C40)/(A42-A40)</f>
+        <f t="shared" si="1"/>
         <v>3.1932203389830514E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>0.8186666666666671</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>37953</v>
       </c>
@@ -17526,15 +17653,19 @@
         <v>18.2</v>
       </c>
       <c r="C42">
-        <f>AVERAGE(B35:B49)</f>
+        <f t="shared" si="3"/>
         <v>16.186</v>
       </c>
       <c r="D42">
-        <f>(C43-C41)/(A43-A41)</f>
+        <f t="shared" ref="D42:D73" si="4">(C43-C41)/(A43-A41)</f>
         <v>3.3387978142076509E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>1.0653333333333332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>37986</v>
       </c>
@@ -17542,15 +17673,19 @@
         <v>18.850000000000001</v>
       </c>
       <c r="C43">
-        <f>AVERAGE(B36:B50)</f>
+        <f t="shared" si="3"/>
         <v>17.157333333333334</v>
       </c>
       <c r="D43">
-        <f>(C44-C42)/(A44-A42)</f>
+        <f t="shared" si="4"/>
         <v>2.812698412698416E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>0.97133333333333383</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>38016</v>
       </c>
@@ -17558,15 +17693,19 @@
         <v>17.46</v>
       </c>
       <c r="C44">
-        <f>AVERAGE(B37:B51)</f>
+        <f t="shared" si="3"/>
         <v>17.958000000000002</v>
       </c>
       <c r="D44">
-        <f>(C45-C43)/(A45-A43)</f>
+        <f t="shared" si="4"/>
         <v>2.6045977011494234E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>0.80066666666666819</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>38044</v>
       </c>
@@ -17574,15 +17713,19 @@
         <v>18.61</v>
       </c>
       <c r="C45">
-        <f>AVERAGE(B38:B52)</f>
+        <f t="shared" si="3"/>
         <v>18.667999999999999</v>
       </c>
       <c r="D45">
-        <f>(C46-C44)/(A46-A44)</f>
+        <f t="shared" si="4"/>
         <v>2.0579234972677527E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>0.7099999999999973</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>38077</v>
       </c>
@@ -17590,15 +17733,19 @@
         <v>17.55</v>
       </c>
       <c r="C46">
-        <f>AVERAGE(B39:B53)</f>
+        <f t="shared" si="3"/>
         <v>19.213333333333331</v>
       </c>
       <c r="D46">
-        <f>(C47-C45)/(A47-A45)</f>
+        <f t="shared" si="4"/>
         <v>1.7492063492063496E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>0.54533333333333189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>38107</v>
       </c>
@@ -17606,15 +17753,19 @@
         <v>21.1</v>
       </c>
       <c r="C47">
-        <f>AVERAGE(B40:B54)</f>
+        <f t="shared" si="3"/>
         <v>19.77</v>
       </c>
       <c r="D47">
-        <f>(C48-C46)/(A48-A46)</f>
+        <f t="shared" si="4"/>
         <v>1.8032786885245924E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>0.55666666666666842</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>38138</v>
       </c>
@@ -17622,15 +17773,19 @@
         <v>20.350000000000001</v>
       </c>
       <c r="C48">
-        <f>AVERAGE(B41:B55)</f>
+        <f t="shared" si="3"/>
         <v>20.313333333333333</v>
       </c>
       <c r="D48">
-        <f>(C49-C47)/(A49-A47)</f>
+        <f t="shared" si="4"/>
         <v>1.5409836065573675E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>0.543333333333333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>38168</v>
       </c>
@@ -17638,15 +17793,19 @@
         <v>22.88</v>
       </c>
       <c r="C49">
-        <f>AVERAGE(B42:B56)</f>
+        <f t="shared" si="3"/>
         <v>20.709999999999994</v>
       </c>
       <c r="D49">
-        <f>(C50-C48)/(A50-A48)</f>
+        <f t="shared" si="4"/>
         <v>1.2766666666666697E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>0.39666666666666117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>38198</v>
       </c>
@@ -17654,15 +17813,19 @@
         <v>22.9</v>
       </c>
       <c r="C50">
-        <f>AVERAGE(B43:B57)</f>
+        <f t="shared" si="3"/>
         <v>21.079333333333334</v>
       </c>
       <c r="D50">
-        <f>(C51-C49)/(A51-A49)</f>
+        <f t="shared" si="4"/>
         <v>1.0483870967742026E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0.36933333333334062</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>38230</v>
       </c>
@@ -17670,15 +17833,19 @@
         <v>21.48</v>
       </c>
       <c r="C51">
-        <f>AVERAGE(B44:B58)</f>
+        <f t="shared" si="3"/>
         <v>21.36</v>
       </c>
       <c r="D51">
-        <f>(C52-C50)/(A52-A50)</f>
+        <f t="shared" si="4"/>
         <v>9.3655913978494473E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0.28066666666666507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>38260</v>
       </c>
@@ -17686,15 +17853,19 @@
         <v>21.33</v>
       </c>
       <c r="C52">
-        <f>AVERAGE(B45:B59)</f>
+        <f t="shared" si="3"/>
         <v>21.66</v>
       </c>
       <c r="D52">
-        <f>(C53-C51)/(A53-A51)</f>
+        <f t="shared" si="4"/>
         <v>1.1209039548022508E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0.30000000000000071</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>38289</v>
       </c>
@@ -17702,15 +17873,19 @@
         <v>22.35</v>
       </c>
       <c r="C53">
-        <f>AVERAGE(B46:B60)</f>
+        <f t="shared" si="3"/>
         <v>22.021333333333327</v>
       </c>
       <c r="D53">
-        <f>(C54-C52)/(A54-A52)</f>
+        <f t="shared" si="4"/>
         <v>1.5540983606557384E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0.36133333333332729</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="1">
         <v>38321</v>
       </c>
@@ -17718,15 +17893,19 @@
         <v>22.75</v>
       </c>
       <c r="C54">
-        <f>AVERAGE(B47:B61)</f>
+        <f t="shared" si="3"/>
         <v>22.608000000000001</v>
       </c>
       <c r="D54">
-        <f>(C55-C53)/(A55-A53)</f>
+        <f t="shared" si="4"/>
         <v>1.6328042328042434E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0.58666666666667311</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="1">
         <v>38352</v>
       </c>
@@ -17734,15 +17913,19 @@
         <v>21.39</v>
       </c>
       <c r="C55">
-        <f>AVERAGE(B48:B62)</f>
+        <f t="shared" si="3"/>
         <v>23.05</v>
       </c>
       <c r="D55">
-        <f>(C56-C54)/(A56-A54)</f>
+        <f t="shared" si="4"/>
         <v>1.4666666666666713E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0.44200000000000017</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="1">
         <v>38383</v>
       </c>
@@ -17750,15 +17933,19 @@
         <v>23.45</v>
       </c>
       <c r="C56">
-        <f>AVERAGE(B49:B63)</f>
+        <f t="shared" si="3"/>
         <v>23.517333333333337</v>
       </c>
       <c r="D56">
-        <f>(C57-C55)/(A57-A55)</f>
+        <f t="shared" si="4"/>
         <v>1.540112994350286E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0.46733333333333604</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1">
         <v>38411</v>
       </c>
@@ -17766,15 +17953,19 @@
         <v>23.74</v>
       </c>
       <c r="C57">
-        <f>AVERAGE(B50:B64)</f>
+        <f t="shared" si="3"/>
         <v>23.958666666666669</v>
       </c>
       <c r="D57">
-        <f>(C58-C56)/(A58-A56)</f>
+        <f t="shared" si="4"/>
         <v>1.4259887005649683E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0.44133333333333269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1">
         <v>38442</v>
       </c>
@@ -17782,15 +17973,19 @@
         <v>23.06</v>
       </c>
       <c r="C58">
-        <f>AVERAGE(B51:B65)</f>
+        <f t="shared" si="3"/>
         <v>24.358666666666668</v>
       </c>
       <c r="D58">
-        <f>(C59-C57)/(A59-A57)</f>
+        <f t="shared" si="4"/>
         <v>1.7722222222222209E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0.39999999999999858</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1">
         <v>38471</v>
       </c>
@@ -17798,15 +17993,19 @@
         <v>21.96</v>
       </c>
       <c r="C59">
-        <f>AVERAGE(B52:B66)</f>
+        <f t="shared" si="3"/>
         <v>25.022000000000002</v>
       </c>
       <c r="D59">
-        <f>(C60-C58)/(A60-A58)</f>
+        <f t="shared" si="4"/>
         <v>2.2426229508196699E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0.663333333333334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="1">
         <v>38503</v>
       </c>
@@ -17814,15 +18013,19 @@
         <v>24.03</v>
       </c>
       <c r="C60">
-        <f>AVERAGE(B53:B67)</f>
+        <f t="shared" si="3"/>
         <v>25.726666666666667</v>
       </c>
       <c r="D60">
-        <f>(C61-C59)/(A61-A59)</f>
+        <f t="shared" si="4"/>
         <v>2.2010752688171955E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0.70466666666666455</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="1">
         <v>38533</v>
       </c>
@@ -17830,15 +18033,19 @@
         <v>26.35</v>
       </c>
       <c r="C61">
-        <f>AVERAGE(B54:B68)</f>
+        <f t="shared" si="3"/>
         <v>26.386666666666663</v>
       </c>
       <c r="D61">
-        <f>(C62-C60)/(A62-A60)</f>
+        <f t="shared" si="4"/>
         <v>2.0237288135593143E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0.65999999999999659</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="1">
         <v>38562</v>
       </c>
@@ -17846,15 +18053,19 @@
         <v>27.73</v>
       </c>
       <c r="C62">
-        <f>AVERAGE(B55:B69)</f>
+        <f t="shared" si="3"/>
         <v>26.920666666666662</v>
       </c>
       <c r="D62">
-        <f>(C63-C61)/(A63-A61)</f>
+        <f t="shared" si="4"/>
         <v>2.2999999999999975E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0.53399999999999892</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="1">
         <v>38595</v>
       </c>
@@ -17862,15 +18073,19 @@
         <v>27.36</v>
       </c>
       <c r="C63">
-        <f>AVERAGE(B56:B70)</f>
+        <f t="shared" si="3"/>
         <v>27.812666666666662</v>
       </c>
       <c r="D63">
-        <f>(C64-C62)/(A64-A62)</f>
+        <f t="shared" si="4"/>
         <v>2.2444444444444354E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0.89199999999999946</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="1">
         <v>38625</v>
       </c>
@@ -17878,15 +18093,19 @@
         <v>29.5</v>
       </c>
       <c r="C64">
-        <f>AVERAGE(B57:B71)</f>
+        <f t="shared" si="3"/>
         <v>28.334666666666656</v>
       </c>
       <c r="D64">
-        <f>(C65-C63)/(A65-A63)</f>
+        <f t="shared" si="4"/>
         <v>1.2994535519125723E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>0.52199999999999491</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="1">
         <v>38656</v>
       </c>
@@ -17894,15 +18113,19 @@
         <v>28.9</v>
       </c>
       <c r="C65">
-        <f>AVERAGE(B58:B72)</f>
+        <f t="shared" si="3"/>
         <v>28.605333333333331</v>
       </c>
       <c r="D65">
-        <f>(C66-C64)/(A66-A64)</f>
+        <f t="shared" si="4"/>
         <v>3.7814207650275176E-3</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>0.27066666666667416</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="1">
         <v>38686</v>
       </c>
@@ -17910,15 +18133,19 @@
         <v>31.43</v>
       </c>
       <c r="C66">
-        <f>AVERAGE(B59:B73)</f>
+        <f t="shared" si="3"/>
         <v>28.565333333333335</v>
       </c>
       <c r="D66">
-        <f>(C67-C65)/(A67-A65)</f>
+        <f t="shared" si="4"/>
         <v>-1.1111111111065479E-5</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>-3.9999999999995595E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="1">
         <v>38716</v>
       </c>
@@ -17926,15 +18153,19 @@
         <v>31.9</v>
       </c>
       <c r="C67">
-        <f>AVERAGE(B60:B74)</f>
+        <f t="shared" si="3"/>
         <v>28.604666666666667</v>
       </c>
       <c r="D67">
-        <f>(C68-C66)/(A68-A66)</f>
+        <f t="shared" si="4"/>
         <v>1.0752688172044691E-4</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>3.9333333333331666E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="1">
         <v>38748</v>
       </c>
@@ -17942,15 +18173,19 @@
         <v>32.25</v>
       </c>
       <c r="C68">
-        <f>AVERAGE(B61:B75)</f>
+        <f t="shared" si="3"/>
         <v>28.572000000000003</v>
       </c>
       <c r="D68">
-        <f>(C69-C67)/(A69-A67)</f>
+        <f t="shared" si="4"/>
         <v>-4.6222222222221864E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>-3.2666666666663957E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="1">
         <v>38776</v>
       </c>
@@ -17958,15 +18193,19 @@
         <v>30.76</v>
       </c>
       <c r="C69">
-        <f>AVERAGE(B62:B76)</f>
+        <f t="shared" si="3"/>
         <v>28.327333333333335</v>
       </c>
       <c r="D69">
-        <f>(C70-C68)/(A70-A68)</f>
+        <f t="shared" si="4"/>
         <v>-1.1468926553672362E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69">
+        <f t="shared" si="2"/>
+        <v>-0.24466666666666725</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="1">
         <v>38807</v>
       </c>
@@ -17974,15 +18213,19 @@
         <v>34.770000000000003</v>
       </c>
       <c r="C70">
-        <f>AVERAGE(B63:B77)</f>
+        <f t="shared" si="3"/>
         <v>27.895333333333333</v>
       </c>
       <c r="D70">
-        <f>(C71-C69)/(A71-A69)</f>
+        <f t="shared" si="4"/>
         <v>-1.314124293785315E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70">
+        <f t="shared" si="2"/>
+        <v>-0.43200000000000216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="1">
         <v>38835</v>
       </c>
@@ -17990,15 +18233,19 @@
         <v>31.28</v>
       </c>
       <c r="C71">
-        <f>AVERAGE(B64:B78)</f>
+        <f t="shared" si="3"/>
         <v>27.552</v>
       </c>
       <c r="D71">
-        <f>(C72-C70)/(A72-A70)</f>
+        <f t="shared" si="4"/>
         <v>-9.3442622950819128E-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71">
+        <f t="shared" si="2"/>
+        <v>-0.34333333333333371</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="1">
         <v>38868</v>
       </c>
@@ -18006,15 +18253,19 @@
         <v>27.8</v>
       </c>
       <c r="C72">
-        <f>AVERAGE(B65:B79)</f>
+        <f t="shared" si="3"/>
         <v>27.325333333333337</v>
       </c>
       <c r="D72">
-        <f>(C73-C71)/(A73-A71)</f>
+        <f t="shared" si="4"/>
         <v>-7.2380952380951737E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72">
+        <f t="shared" si="2"/>
+        <v>-0.22666666666666302</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="1">
         <v>38898</v>
       </c>
@@ -18022,15 +18273,19 @@
         <v>22.46</v>
       </c>
       <c r="C73">
-        <f>AVERAGE(B66:B80)</f>
+        <f t="shared" ref="C73:C104" si="5">AVERAGE(B66:B80)</f>
         <v>27.096000000000004</v>
       </c>
       <c r="D73">
-        <f>(C74-C72)/(A74-A72)</f>
+        <f t="shared" si="4"/>
         <v>-9.7923497267759264E-3</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73">
+        <f t="shared" si="2"/>
+        <v>-0.22933333333333294</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="1">
         <v>38929</v>
       </c>
@@ -18038,15 +18293,19 @@
         <v>22.55</v>
       </c>
       <c r="C74">
-        <f>AVERAGE(B67:B81)</f>
+        <f t="shared" si="5"/>
         <v>26.728000000000005</v>
       </c>
       <c r="D74">
-        <f>(C75-C73)/(A75-A73)</f>
+        <f t="shared" ref="D74:D105" si="6">(C75-C73)/(A75-A73)</f>
         <v>-1.5268817204301113E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74">
+        <f t="shared" si="2"/>
+        <v>-0.36799999999999855</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="1">
         <v>38960</v>
       </c>
@@ -18054,15 +18313,19 @@
         <v>23.54</v>
       </c>
       <c r="C75">
-        <f>AVERAGE(B68:B82)</f>
+        <f t="shared" si="5"/>
         <v>26.149333333333335</v>
       </c>
       <c r="D75">
-        <f>(C76-C74)/(A76-A74)</f>
+        <f t="shared" si="6"/>
         <v>-1.9122222222222263E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75">
+        <f t="shared" ref="E75:E138" si="7">C75-C74</f>
+        <v>-0.57866666666667044</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="1">
         <v>38989</v>
       </c>
@@ -18070,15 +18333,19 @@
         <v>22.68</v>
       </c>
       <c r="C76">
-        <f>AVERAGE(B69:B83)</f>
+        <f t="shared" si="5"/>
         <v>25.580666666666669</v>
       </c>
       <c r="D76">
-        <f>(C77-C75)/(A77-A75)</f>
+        <f t="shared" si="6"/>
         <v>-1.7398907103825086E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76">
+        <f t="shared" si="7"/>
+        <v>-0.56866666666666532</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="1">
         <v>39021</v>
       </c>
@@ -18086,15 +18353,19 @@
         <v>21.25</v>
       </c>
       <c r="C77">
-        <f>AVERAGE(B70:B84)</f>
+        <f t="shared" si="5"/>
         <v>25.088000000000005</v>
       </c>
       <c r="D77">
-        <f>(C78-C76)/(A78-A76)</f>
+        <f t="shared" si="6"/>
         <v>-1.9397849462365575E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77">
+        <f t="shared" si="7"/>
+        <v>-0.49266666666666481</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="1">
         <v>39051</v>
       </c>
@@ -18102,15 +18373,19 @@
         <v>22.21</v>
       </c>
       <c r="C78">
-        <f>AVERAGE(B71:B85)</f>
+        <f t="shared" si="5"/>
         <v>24.378000000000004</v>
       </c>
       <c r="D78">
-        <f>(C79-C77)/(A79-A77)</f>
+        <f t="shared" si="6"/>
         <v>-2.2214689265536835E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78">
+        <f t="shared" si="7"/>
+        <v>-0.71000000000000085</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="1">
         <v>39080</v>
       </c>
@@ -18118,15 +18393,19 @@
         <v>26.1</v>
       </c>
       <c r="C79">
-        <f>AVERAGE(B72:B86)</f>
+        <f t="shared" si="5"/>
         <v>23.777333333333331</v>
       </c>
       <c r="D79">
-        <f>(C80-C78)/(A80-A78)</f>
+        <f t="shared" si="6"/>
         <v>-1.6161290322580742E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <f t="shared" si="7"/>
+        <v>-0.60066666666667246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="1">
         <v>39113</v>
       </c>
@@ -18134,15 +18413,19 @@
         <v>25.46</v>
       </c>
       <c r="C80">
-        <f>AVERAGE(B73:B87)</f>
+        <f t="shared" si="5"/>
         <v>23.375999999999998</v>
       </c>
       <c r="D80">
-        <f>(C81-C79)/(A81-A79)</f>
+        <f t="shared" si="6"/>
         <v>-7.5628415300546857E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80">
+        <f t="shared" si="7"/>
+        <v>-0.40133333333333354</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="1">
         <v>39141</v>
       </c>
@@ -18150,15 +18433,19 @@
         <v>25.91</v>
       </c>
       <c r="C81">
-        <f>AVERAGE(B74:B88)</f>
+        <f t="shared" si="5"/>
         <v>23.315999999999995</v>
       </c>
       <c r="D81">
-        <f>(C82-C80)/(A82-A80)</f>
+        <f t="shared" si="6"/>
         <v>-1.1494252873516011E-5</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81">
+        <f t="shared" si="7"/>
+        <v>-6.0000000000002274E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="1">
         <v>39171</v>
       </c>
@@ -18166,15 +18453,19 @@
         <v>23.22</v>
       </c>
       <c r="C82">
-        <f>AVERAGE(B75:B89)</f>
+        <f t="shared" si="5"/>
         <v>23.375333333333334</v>
       </c>
       <c r="D82">
-        <f>(C83-C81)/(A83-A81)</f>
+        <f t="shared" si="6"/>
         <v>-7.7595628415290548E-4</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82">
+        <f t="shared" si="7"/>
+        <v>5.9333333333338345E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="1">
         <v>39202</v>
       </c>
@@ -18182,15 +18473,19 @@
         <v>23.72</v>
       </c>
       <c r="C83">
-        <f>AVERAGE(B76:B90)</f>
+        <f t="shared" si="5"/>
         <v>23.268666666666668</v>
       </c>
       <c r="D83">
-        <f>(C84-C82)/(A84-A82)</f>
+        <f t="shared" si="6"/>
         <v>-2.6344086021505481E-3</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83">
+        <f t="shared" si="7"/>
+        <v>-0.10666666666666558</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="1">
         <v>39233</v>
       </c>
@@ -18198,15 +18493,19 @@
         <v>23.37</v>
       </c>
       <c r="C84">
-        <f>AVERAGE(B77:B91)</f>
+        <f t="shared" si="5"/>
         <v>23.212</v>
       </c>
       <c r="D84">
-        <f>(C85-C83)/(A85-A83)</f>
+        <f t="shared" si="6"/>
         <v>-5.6222222222222246E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84">
+        <f t="shared" si="7"/>
+        <v>-5.6666666666668419E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="1">
         <v>39262</v>
       </c>
@@ -18214,15 +18513,19 @@
         <v>24.12</v>
       </c>
       <c r="C85">
-        <f>AVERAGE(B78:B92)</f>
+        <f t="shared" si="5"/>
         <v>22.931333333333335</v>
       </c>
       <c r="D85">
-        <f>(C86-C84)/(A86-A84)</f>
+        <f t="shared" si="6"/>
         <v>-9.8251366120218099E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85">
+        <f t="shared" si="7"/>
+        <v>-0.28066666666666507</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="1">
         <v>39294</v>
       </c>
@@ -18230,15 +18533,19 @@
         <v>22.27</v>
       </c>
       <c r="C86">
-        <f>AVERAGE(B79:B93)</f>
+        <f t="shared" si="5"/>
         <v>22.612666666666669</v>
       </c>
       <c r="D86">
-        <f>(C87-C85)/(A87-A85)</f>
+        <f t="shared" si="6"/>
         <v>-1.6793650793650791E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86">
+        <f t="shared" si="7"/>
+        <v>-0.31866666666666532</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="1">
         <v>39325</v>
       </c>
@@ -18246,15 +18553,19 @@
         <v>21.78</v>
       </c>
       <c r="C87">
-        <f>AVERAGE(B80:B94)</f>
+        <f t="shared" si="5"/>
         <v>21.873333333333335</v>
       </c>
       <c r="D87">
-        <f>(C88-C86)/(A88-A86)</f>
+        <f t="shared" si="6"/>
         <v>-2.3050847457627168E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87">
+        <f t="shared" si="7"/>
+        <v>-0.73933333333333451</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="1">
         <v>39353</v>
       </c>
@@ -18262,15 +18573,19 @@
         <v>21.56</v>
       </c>
       <c r="C88">
-        <f>AVERAGE(B81:B95)</f>
+        <f t="shared" si="5"/>
         <v>21.252666666666666</v>
       </c>
       <c r="D88">
-        <f>(C89-C87)/(A89-A87)</f>
+        <f t="shared" si="6"/>
         <v>-2.2076502732240568E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88">
+        <f t="shared" si="7"/>
+        <v>-0.62066666666666848</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="1">
         <v>39386</v>
       </c>
@@ -18278,15 +18593,19 @@
         <v>23.44</v>
       </c>
       <c r="C89">
-        <f>AVERAGE(B82:B96)</f>
+        <f t="shared" si="5"/>
         <v>20.52666666666666</v>
       </c>
       <c r="D89">
-        <f>(C90-C88)/(A90-A88)</f>
+        <f t="shared" si="6"/>
         <v>-2.3354497354497364E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89">
+        <f t="shared" si="7"/>
+        <v>-0.7260000000000062</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="1">
         <v>39416</v>
       </c>
@@ -18294,15 +18613,19 @@
         <v>21.94</v>
       </c>
       <c r="C90">
-        <f>AVERAGE(B83:B97)</f>
+        <f t="shared" si="5"/>
         <v>19.781333333333333</v>
       </c>
       <c r="D90">
-        <f>(C91-C89)/(A91-A89)</f>
+        <f t="shared" si="6"/>
         <v>-2.4819672131147413E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90">
+        <f t="shared" si="7"/>
+        <v>-0.74533333333332763</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="1">
         <v>39447</v>
       </c>
@@ -18310,15 +18633,19 @@
         <v>21.83</v>
       </c>
       <c r="C91">
-        <f>AVERAGE(B84:B98)</f>
+        <f t="shared" si="5"/>
         <v>19.012666666666668</v>
       </c>
       <c r="D91">
-        <f>(C92-C90)/(A92-A90)</f>
+        <f t="shared" si="6"/>
         <v>-2.1043010752688159E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91">
+        <f t="shared" si="7"/>
+        <v>-0.76866666666666461</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="1">
         <v>39478</v>
       </c>
@@ -18326,15 +18653,19 @@
         <v>17.04</v>
       </c>
       <c r="C92">
-        <f>AVERAGE(B85:B99)</f>
+        <f t="shared" si="5"/>
         <v>18.476666666666667</v>
       </c>
       <c r="D92">
-        <f>(C93-C91)/(A93-A91)</f>
+        <f t="shared" si="6"/>
         <v>-2.240000000000008E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92">
+        <f t="shared" si="7"/>
+        <v>-0.53600000000000136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="1">
         <v>39507</v>
       </c>
@@ -18342,15 +18673,19 @@
         <v>17.43</v>
       </c>
       <c r="C93">
-        <f>AVERAGE(B86:B100)</f>
+        <f t="shared" si="5"/>
         <v>17.668666666666663</v>
       </c>
       <c r="D93">
-        <f>(C94-C92)/(A94-A92)</f>
+        <f t="shared" si="6"/>
         <v>-2.3833333333333328E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93">
+        <f t="shared" si="7"/>
+        <v>-0.80800000000000338</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="1">
         <v>39538</v>
       </c>
@@ -18358,15 +18693,19 @@
         <v>15.01</v>
       </c>
       <c r="C94">
-        <f>AVERAGE(B87:B101)</f>
+        <f t="shared" si="5"/>
         <v>17.046666666666667</v>
       </c>
       <c r="D94">
-        <f>(C95-C93)/(A95-A93)</f>
+        <f t="shared" si="6"/>
         <v>-2.0382513661202112E-2</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94">
+        <f t="shared" si="7"/>
+        <v>-0.62199999999999633</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="1">
         <v>39568</v>
       </c>
@@ -18374,15 +18713,19 @@
         <v>16.149999999999999</v>
       </c>
       <c r="C95">
-        <f>AVERAGE(B88:B102)</f>
+        <f t="shared" si="5"/>
         <v>16.425333333333334</v>
       </c>
       <c r="D95">
-        <f>(C96-C94)/(A96-A94)</f>
+        <f t="shared" si="6"/>
         <v>-2.0944444444444432E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95">
+        <f t="shared" si="7"/>
+        <v>-0.6213333333333324</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="1">
         <v>39598</v>
       </c>
@@ -18390,15 +18733,19 @@
         <v>15.02</v>
       </c>
       <c r="C96">
-        <f>AVERAGE(B89:B103)</f>
+        <f t="shared" si="5"/>
         <v>15.790000000000001</v>
       </c>
       <c r="D96">
-        <f>(C97-C95)/(A97-A95)</f>
+        <f t="shared" si="6"/>
         <v>-2.105464480874316E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96">
+        <f t="shared" si="7"/>
+        <v>-0.63533333333333353</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="1">
         <v>39629</v>
       </c>
@@ -18406,15 +18753,19 @@
         <v>12.04</v>
       </c>
       <c r="C97">
-        <f>AVERAGE(B90:B104)</f>
+        <f t="shared" si="5"/>
         <v>15.141000000000002</v>
       </c>
       <c r="D97">
-        <f>(C98-C96)/(A98-A96)</f>
+        <f t="shared" si="6"/>
         <v>-2.1521505376344056E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97">
+        <f t="shared" si="7"/>
+        <v>-0.64899999999999913</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="1">
         <v>39660</v>
       </c>
@@ -18422,15 +18773,19 @@
         <v>12.19</v>
       </c>
       <c r="C98">
-        <f>AVERAGE(B91:B105)</f>
+        <f t="shared" si="5"/>
         <v>14.455666666666669</v>
       </c>
       <c r="D98">
-        <f>(C99-C97)/(A99-A97)</f>
+        <f t="shared" si="6"/>
         <v>-2.5944444444444503E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98">
+        <f t="shared" si="7"/>
+        <v>-0.68533333333333246</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="1">
         <v>39689</v>
       </c>
@@ -18438,15 +18793,19 @@
         <v>15.33</v>
       </c>
       <c r="C99">
-        <f>AVERAGE(B92:B106)</f>
+        <f t="shared" si="5"/>
         <v>13.584333333333332</v>
       </c>
       <c r="D99">
-        <f>(C100-C98)/(A100-A98)</f>
+        <f t="shared" si="6"/>
         <v>-2.0885245901639361E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99">
+        <f t="shared" si="7"/>
+        <v>-0.87133333333333773</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="1">
         <v>39721</v>
       </c>
@@ -18454,15 +18813,19 @@
         <v>12</v>
       </c>
       <c r="C100">
-        <f>AVERAGE(B93:B107)</f>
+        <f t="shared" si="5"/>
         <v>13.181666666666668</v>
       </c>
       <c r="D100">
-        <f>(C101-C99)/(A101-A99)</f>
+        <f t="shared" si="6"/>
         <v>-1.2714285714285688E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100">
+        <f t="shared" si="7"/>
+        <v>-0.40266666666666318</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="1">
         <v>39752</v>
       </c>
@@ -18470,15 +18833,19 @@
         <v>12.94</v>
       </c>
       <c r="C101">
-        <f>AVERAGE(B94:B108)</f>
+        <f t="shared" si="5"/>
         <v>12.783333333333333</v>
       </c>
       <c r="D101">
-        <f>(C102-C100)/(A102-A100)</f>
+        <f t="shared" si="6"/>
         <v>-1.0706214689265555E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101">
+        <f t="shared" si="7"/>
+        <v>-0.3983333333333352</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="1">
         <v>39780</v>
       </c>
@@ -18486,15 +18853,19 @@
         <v>12.46</v>
       </c>
       <c r="C102">
-        <f>AVERAGE(B95:B109)</f>
+        <f t="shared" si="5"/>
         <v>12.55</v>
       </c>
       <c r="D102">
-        <f>(C103-C101)/(A103-A101)</f>
+        <f t="shared" si="6"/>
         <v>-6.8524590163934595E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102">
+        <f t="shared" si="7"/>
+        <v>-0.2333333333333325</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="1">
         <v>39813</v>
       </c>
@@ -18502,15 +18873,19 @@
         <v>12.03</v>
       </c>
       <c r="C103">
-        <f>AVERAGE(B96:B110)</f>
+        <f t="shared" si="5"/>
         <v>12.365333333333332</v>
       </c>
       <c r="D103">
-        <f>(C104-C102)/(A104-A102)</f>
+        <f t="shared" si="6"/>
         <v>-3.5238095238095163E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103">
+        <f t="shared" si="7"/>
+        <v>-0.18466666666666853</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="1">
         <v>39843</v>
       </c>
@@ -18518,15 +18893,19 @@
         <v>13.705</v>
       </c>
       <c r="C104">
-        <f>AVERAGE(B97:B111)</f>
+        <f t="shared" si="5"/>
         <v>12.328000000000001</v>
       </c>
       <c r="D104">
-        <f>(C105-C103)/(A105-A103)</f>
+        <f t="shared" si="6"/>
         <v>3.1551724137931312E-3</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="E104">
+        <f t="shared" si="7"/>
+        <v>-3.7333333333330998E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="1">
         <v>39871</v>
       </c>
@@ -18534,15 +18913,19 @@
         <v>11.66</v>
       </c>
       <c r="C105">
-        <f>AVERAGE(B98:B112)</f>
+        <f t="shared" ref="C105:C136" si="8">AVERAGE(B98:B112)</f>
         <v>12.548333333333334</v>
       </c>
       <c r="D105">
-        <f>(C106-C104)/(A106-A104)</f>
+        <f t="shared" si="6"/>
         <v>4.3333333333333002E-3</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105">
+        <f t="shared" si="7"/>
+        <v>0.2203333333333326</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="1">
         <v>39903</v>
       </c>
@@ -18550,15 +18933,19 @@
         <v>8.76</v>
       </c>
       <c r="C106">
-        <f>AVERAGE(B99:B113)</f>
+        <f t="shared" si="8"/>
         <v>12.587999999999999</v>
       </c>
       <c r="D106">
-        <f>(C107-C105)/(A107-A105)</f>
+        <f t="shared" ref="D106:D137" si="9">(C107-C105)/(A107-A105)</f>
         <v>-3.0322580645161389E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106">
+        <f t="shared" si="7"/>
+        <v>3.9666666666665407E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="1">
         <v>39933</v>
       </c>
@@ -18566,15 +18953,19 @@
         <v>11</v>
       </c>
       <c r="C107">
-        <f>AVERAGE(B100:B114)</f>
+        <f t="shared" si="8"/>
         <v>12.360333333333333</v>
       </c>
       <c r="D107">
-        <f>(C108-C106)/(A108-A106)</f>
+        <f t="shared" si="9"/>
         <v>-1.5028248587570321E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107">
+        <f t="shared" si="7"/>
+        <v>-0.22766666666666602</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="1">
         <v>39962</v>
       </c>
@@ -18582,15 +18973,19 @@
         <v>11.455</v>
       </c>
       <c r="C108">
-        <f>AVERAGE(B101:B115)</f>
+        <f t="shared" si="8"/>
         <v>12.499333333333334</v>
       </c>
       <c r="D108">
-        <f>(C109-C107)/(A109-A107)</f>
+        <f t="shared" si="9"/>
         <v>3.655737704918045E-3</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108">
+        <f t="shared" si="7"/>
+        <v>0.13900000000000112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="1">
         <v>39994</v>
       </c>
@@ -18598,15 +18993,19 @@
         <v>11.51</v>
       </c>
       <c r="C109">
-        <f>AVERAGE(B102:B116)</f>
+        <f t="shared" si="8"/>
         <v>12.583333333333334</v>
       </c>
       <c r="D109">
-        <f>(C110-C108)/(A110-A108)</f>
+        <f t="shared" si="9"/>
         <v>4.1851851851851685E-3</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109">
+        <f t="shared" si="7"/>
+        <v>8.3999999999999631E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="1">
         <v>40025</v>
       </c>
@@ -18614,15 +19013,19 @@
         <v>13.38</v>
       </c>
       <c r="C110">
-        <f>AVERAGE(B103:B117)</f>
+        <f t="shared" si="8"/>
         <v>12.763</v>
       </c>
       <c r="D110">
-        <f>(C111-C109)/(A111-A109)</f>
+        <f t="shared" si="9"/>
         <v>5.9784946236559142E-3</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110">
+        <f t="shared" si="7"/>
+        <v>0.17966666666666598</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="1">
         <v>40056</v>
       </c>
@@ -18630,15 +19033,19 @@
         <v>14.46</v>
       </c>
       <c r="C111">
-        <f>AVERAGE(B104:B118)</f>
+        <f t="shared" si="8"/>
         <v>12.954000000000001</v>
       </c>
       <c r="D111">
-        <f>(C112-C110)/(A112-A110)</f>
+        <f t="shared" si="9"/>
         <v>3.4863387978141878E-3</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="E111">
+        <f t="shared" si="7"/>
+        <v>0.19100000000000072</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="1">
         <v>40086</v>
       </c>
@@ -18646,15 +19053,19 @@
         <v>15.345000000000001</v>
       </c>
       <c r="C112">
-        <f>AVERAGE(B105:B119)</f>
+        <f t="shared" si="8"/>
         <v>12.975666666666665</v>
       </c>
       <c r="D112">
-        <f>(C113-C111)/(A113-A111)</f>
+        <f t="shared" si="9"/>
         <v>5.5055555555555335E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112">
+        <f t="shared" si="7"/>
+        <v>2.1666666666664725E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="1">
         <v>40116</v>
       </c>
@@ -18662,15 +19073,19 @@
         <v>12.785</v>
       </c>
       <c r="C113">
-        <f>AVERAGE(B106:B120)</f>
+        <f t="shared" si="8"/>
         <v>13.284333333333333</v>
       </c>
       <c r="D113">
-        <f>(C114-C112)/(A114-A112)</f>
+        <f t="shared" si="9"/>
         <v>1.3923497267759573E-2</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113">
+        <f t="shared" si="7"/>
+        <v>0.30866666666666731</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="1">
         <v>40147</v>
       </c>
@@ -18678,15 +19093,19 @@
         <v>11.914999999999999</v>
       </c>
       <c r="C114">
-        <f>AVERAGE(B107:B121)</f>
+        <f t="shared" si="8"/>
         <v>13.824999999999999</v>
       </c>
       <c r="D114">
-        <f>(C115-C113)/(A115-A113)</f>
+        <f t="shared" si="9"/>
         <v>1.6440860215053772E-2</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114">
+        <f t="shared" si="7"/>
+        <v>0.54066666666666663</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="1">
         <v>40178</v>
       </c>
@@ -18694,15 +19113,19 @@
         <v>14.085000000000001</v>
       </c>
       <c r="C115">
-        <f>AVERAGE(B108:B122)</f>
+        <f t="shared" si="8"/>
         <v>14.303666666666667</v>
       </c>
       <c r="D115">
-        <f>(C116-C114)/(A116-A114)</f>
+        <f t="shared" si="9"/>
         <v>1.4544444444444487E-2</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115">
+        <f t="shared" si="7"/>
+        <v>0.47866666666666724</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="1">
         <v>40207</v>
       </c>
@@ -18710,15 +19133,19 @@
         <v>14.2</v>
       </c>
       <c r="C116">
-        <f>AVERAGE(B109:B123)</f>
+        <f t="shared" si="8"/>
         <v>14.697666666666668</v>
       </c>
       <c r="D116">
-        <f>(C117-C115)/(A117-A115)</f>
+        <f t="shared" si="9"/>
         <v>1.4847953216374278E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116">
+        <f t="shared" si="7"/>
+        <v>0.3940000000000019</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="1">
         <v>40235</v>
       </c>
@@ -18726,15 +19153,19 @@
         <v>15.154999999999999</v>
       </c>
       <c r="C117">
-        <f>AVERAGE(B110:B124)</f>
+        <f t="shared" si="8"/>
         <v>15.15</v>
       </c>
       <c r="D117">
-        <f>(C118-C116)/(A118-A116)</f>
+        <f t="shared" si="9"/>
         <v>1.3431693989071E-2</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117">
+        <f t="shared" si="7"/>
+        <v>0.45233333333333192</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="1">
         <v>40268</v>
       </c>
@@ -18742,15 +19173,19 @@
         <v>14.895</v>
       </c>
       <c r="C118">
-        <f>AVERAGE(B111:B125)</f>
+        <f t="shared" si="8"/>
         <v>15.516999999999999</v>
       </c>
       <c r="D118">
-        <f>(C119-C117)/(A119-A117)</f>
+        <f t="shared" si="9"/>
         <v>8.7883597883597862E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118">
+        <f t="shared" si="7"/>
+        <v>0.3669999999999991</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="1">
         <v>40298</v>
       </c>
@@ -18758,15 +19193,19 @@
         <v>14.03</v>
       </c>
       <c r="C119">
-        <f>AVERAGE(B112:B126)</f>
+        <f t="shared" si="8"/>
         <v>15.703666666666667</v>
       </c>
       <c r="D119">
-        <f>(C120-C118)/(A120-A118)</f>
+        <f t="shared" si="9"/>
         <v>5.3497267759562697E-3</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119">
+        <f t="shared" si="7"/>
+        <v>0.18666666666666742</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="1">
         <v>40329</v>
       </c>
@@ -18774,15 +19213,19 @@
         <v>16.29</v>
       </c>
       <c r="C120">
-        <f>AVERAGE(B113:B127)</f>
+        <f t="shared" si="8"/>
         <v>15.843333333333332</v>
       </c>
       <c r="D120">
-        <f>(C121-C119)/(A121-A119)</f>
+        <f t="shared" si="9"/>
         <v>1.1322404371584733E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120">
+        <f t="shared" si="7"/>
+        <v>0.13966666666666505</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="1">
         <v>40359</v>
       </c>
@@ -18790,15 +19233,19 @@
         <v>16.87</v>
       </c>
       <c r="C121">
-        <f>AVERAGE(B114:B128)</f>
+        <f t="shared" si="8"/>
         <v>16.394333333333336</v>
       </c>
       <c r="D121">
-        <f>(C122-C120)/(A122-A120)</f>
+        <f t="shared" si="9"/>
         <v>1.9233333333333363E-2</v>
       </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="E121">
+        <f t="shared" si="7"/>
+        <v>0.55100000000000371</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="1">
         <v>40389</v>
       </c>
@@ -18806,15 +19253,19 @@
         <v>18.18</v>
       </c>
       <c r="C122">
-        <f>AVERAGE(B115:B129)</f>
+        <f t="shared" si="8"/>
         <v>16.997333333333334</v>
       </c>
       <c r="D122">
-        <f>(C123-C121)/(A123-A121)</f>
+        <f t="shared" si="9"/>
         <v>1.6666666666666635E-2</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122">
+        <f t="shared" si="7"/>
+        <v>0.60299999999999798</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="1">
         <v>40421</v>
       </c>
@@ -18822,15 +19273,19 @@
         <v>17.364999999999998</v>
       </c>
       <c r="C123">
-        <f>AVERAGE(B116:B130)</f>
+        <f t="shared" si="8"/>
         <v>17.427666666666667</v>
       </c>
       <c r="D123">
-        <f>(C124-C122)/(A124-A122)</f>
+        <f t="shared" si="9"/>
         <v>1.4134408602150506E-2</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123">
+        <f t="shared" si="7"/>
+        <v>0.43033333333333346</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" s="1">
         <v>40451</v>
       </c>
@@ -18838,15 +19293,19 @@
         <v>18.295000000000002</v>
       </c>
       <c r="C124">
-        <f>AVERAGE(B117:B131)</f>
+        <f t="shared" si="8"/>
         <v>17.873666666666665</v>
       </c>
       <c r="D124">
-        <f>(C125-C123)/(A125-A123)</f>
+        <f t="shared" si="9"/>
         <v>1.6288135593220315E-2</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124">
+        <f t="shared" si="7"/>
+        <v>0.44599999999999795</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="1">
         <v>40480</v>
       </c>
@@ -18854,15 +19313,19 @@
         <v>18.885000000000002</v>
       </c>
       <c r="C125">
-        <f>AVERAGE(B118:B132)</f>
+        <f t="shared" si="8"/>
         <v>18.388666666666666</v>
       </c>
       <c r="D125">
-        <f>(C126-C124)/(A126-A124)</f>
+        <f t="shared" si="9"/>
         <v>1.7387978142076495E-2</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125">
+        <f t="shared" si="7"/>
+        <v>0.51500000000000057</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="1">
         <v>40512</v>
       </c>
@@ -18870,15 +19333,19 @@
         <v>17.260000000000002</v>
       </c>
       <c r="C126">
-        <f>AVERAGE(B119:B133)</f>
+        <f t="shared" si="8"/>
         <v>18.934333333333331</v>
       </c>
       <c r="D126">
-        <f>(C127-C125)/(A127-A125)</f>
+        <f t="shared" si="9"/>
         <v>1.9423280423280419E-2</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126">
+        <f t="shared" si="7"/>
+        <v>0.54566666666666563</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="1">
         <v>40543</v>
       </c>
@@ -18886,15 +19353,19 @@
         <v>17.440000000000001</v>
       </c>
       <c r="C127">
-        <f>AVERAGE(B120:B134)</f>
+        <f t="shared" si="8"/>
         <v>19.612333333333332</v>
       </c>
       <c r="D127">
-        <f>(C128-C126)/(A128-A126)</f>
+        <f t="shared" si="9"/>
         <v>1.7166666666666674E-2</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127">
+        <f t="shared" si="7"/>
+        <v>0.67800000000000082</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="1">
         <v>40574</v>
       </c>
@@ -18902,15 +19373,19 @@
         <v>21.05</v>
       </c>
       <c r="C128">
-        <f>AVERAGE(B121:B135)</f>
+        <f t="shared" si="8"/>
         <v>19.998666666666665</v>
       </c>
       <c r="D128">
-        <f>(C129-C127)/(A129-A127)</f>
+        <f t="shared" si="9"/>
         <v>1.1446327683615778E-2</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128">
+        <f t="shared" si="7"/>
+        <v>0.38633333333333297</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="1">
         <v>40602</v>
       </c>
@@ -18918,15 +19393,19 @@
         <v>20.96</v>
       </c>
       <c r="C129">
-        <f>AVERAGE(B122:B136)</f>
+        <f t="shared" si="8"/>
         <v>20.287666666666663</v>
       </c>
       <c r="D129">
-        <f>(C130-C128)/(A130-A128)</f>
+        <f t="shared" si="9"/>
         <v>8.5028248587570368E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129">
+        <f t="shared" si="7"/>
+        <v>0.28899999999999793</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="1">
         <v>40633</v>
       </c>
@@ -18934,15 +19413,19 @@
         <v>20.54</v>
       </c>
       <c r="C130">
-        <f>AVERAGE(B123:B137)</f>
+        <f t="shared" si="8"/>
         <v>20.50033333333333</v>
       </c>
       <c r="D130">
-        <f>(C131-C129)/(A131-A129)</f>
+        <f t="shared" si="9"/>
         <v>8.9111111111111665E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130">
+        <f t="shared" si="7"/>
+        <v>0.21266666666666723</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="1">
         <v>40662</v>
       </c>
@@ -18950,15 +19433,19 @@
         <v>20.89</v>
       </c>
       <c r="C131">
-        <f>AVERAGE(B124:B138)</f>
+        <f t="shared" si="8"/>
         <v>20.822333333333333</v>
       </c>
       <c r="D131">
-        <f>(C132-C130)/(A132-A130)</f>
+        <f t="shared" si="9"/>
         <v>1.1677595628415303E-2</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="E131">
+        <f t="shared" si="7"/>
+        <v>0.32200000000000273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="1">
         <v>40694</v>
       </c>
@@ -18966,15 +19453,19 @@
         <v>22.88</v>
       </c>
       <c r="C132">
-        <f>AVERAGE(B125:B139)</f>
+        <f t="shared" si="8"/>
         <v>21.212666666666664</v>
       </c>
       <c r="D132">
-        <f>(C133-C131)/(A133-A131)</f>
+        <f t="shared" si="9"/>
         <v>1.3602150537634415E-2</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132">
+        <f t="shared" si="7"/>
+        <v>0.39033333333333076</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="1">
         <v>40724</v>
       </c>
@@ -18982,15 +19473,19 @@
         <v>23.08</v>
       </c>
       <c r="C133">
-        <f>AVERAGE(B126:B140)</f>
+        <f t="shared" si="8"/>
         <v>21.665666666666667</v>
       </c>
       <c r="D133">
-        <f>(C134-C132)/(A134-A132)</f>
+        <f t="shared" si="9"/>
         <v>1.8983050847457644E-2</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133">
+        <f t="shared" si="7"/>
+        <v>0.45300000000000296</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="1">
         <v>40753</v>
       </c>
@@ -18998,15 +19493,19 @@
         <v>24.2</v>
       </c>
       <c r="C134">
-        <f>AVERAGE(B127:B141)</f>
+        <f t="shared" si="8"/>
         <v>22.332666666666665</v>
       </c>
       <c r="D134">
-        <f>(C135-C133)/(A135-A133)</f>
+        <f t="shared" si="9"/>
         <v>2.5021505376344007E-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134">
+        <f t="shared" si="7"/>
+        <v>0.66699999999999804</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="1">
         <v>40786</v>
       </c>
@@ -19014,15 +19513,19 @@
         <v>22.085000000000001</v>
       </c>
       <c r="C135">
-        <f>AVERAGE(B128:B142)</f>
+        <f t="shared" si="8"/>
         <v>23.216999999999995</v>
       </c>
       <c r="D135">
-        <f>(C136-C134)/(A136-A134)</f>
+        <f t="shared" si="9"/>
         <v>2.332275132275129E-2</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135">
+        <f t="shared" si="7"/>
+        <v>0.88433333333333053</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="1">
         <v>40816</v>
       </c>
@@ -19030,15 +19533,19 @@
         <v>21.204999999999998</v>
       </c>
       <c r="C136">
-        <f>AVERAGE(B129:B143)</f>
+        <f t="shared" si="8"/>
         <v>23.801999999999996</v>
       </c>
       <c r="D136">
-        <f>(C137-C135)/(A137-A135)</f>
+        <f t="shared" si="9"/>
         <v>1.626775956284161E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136">
+        <f t="shared" si="7"/>
+        <v>0.58500000000000085</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="1">
         <v>40847</v>
       </c>
@@ -19046,15 +19553,19 @@
         <v>21.37</v>
       </c>
       <c r="C137">
-        <f>AVERAGE(B130:B144)</f>
+        <f t="shared" ref="C137:C168" si="10">AVERAGE(B130:B144)</f>
         <v>24.209333333333333</v>
       </c>
       <c r="D137">
-        <f>(C138-C136)/(A138-A136)</f>
+        <f t="shared" si="9"/>
         <v>1.4765027322404419E-2</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137">
+        <f t="shared" si="7"/>
+        <v>0.40733333333333732</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="1">
         <v>40877</v>
       </c>
@@ -19062,15 +19573,19 @@
         <v>22.195</v>
       </c>
       <c r="C138">
-        <f>AVERAGE(B131:B145)</f>
+        <f t="shared" si="10"/>
         <v>24.702666666666666</v>
       </c>
       <c r="D138">
-        <f>(C139-C137)/(A139-A137)</f>
+        <f t="shared" ref="D138:D164" si="11">(C139-C137)/(A139-A137)</f>
         <v>1.7522222222222203E-2</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138">
+        <f t="shared" si="7"/>
+        <v>0.49333333333333229</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="1">
         <v>40907</v>
       </c>
@@ -19078,15 +19593,19 @@
         <v>24.15</v>
       </c>
       <c r="C139">
-        <f>AVERAGE(B132:B146)</f>
+        <f t="shared" si="10"/>
         <v>25.260666666666665</v>
       </c>
       <c r="D139">
-        <f>(C140-C138)/(A140-A138)</f>
+        <f t="shared" si="11"/>
         <v>1.6999999999999977E-2</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139">
+        <f t="shared" ref="E139:E164" si="12">C139-C138</f>
+        <v>0.55799999999999983</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="1">
         <v>40939</v>
       </c>
@@ -19094,15 +19613,19 @@
         <v>25.68</v>
       </c>
       <c r="C140">
-        <f>AVERAGE(B133:B147)</f>
+        <f t="shared" si="10"/>
         <v>25.756666666666664</v>
       </c>
       <c r="D140">
-        <f>(C141-C139)/(A141-A139)</f>
+        <f t="shared" si="11"/>
         <v>9.8633879781420755E-3</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140">
+        <f t="shared" si="12"/>
+        <v>0.49599999999999866</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="1">
         <v>40968</v>
       </c>
@@ -19110,15 +19633,19 @@
         <v>27.265000000000001</v>
       </c>
       <c r="C141">
-        <f>AVERAGE(B134:B148)</f>
+        <f t="shared" si="10"/>
         <v>25.862333333333332</v>
       </c>
       <c r="D141">
-        <f>(C142-C140)/(A142-A140)</f>
+        <f t="shared" si="11"/>
         <v>5.4180790960451954E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="E141">
+        <f t="shared" si="12"/>
+        <v>0.10566666666666791</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="1">
         <v>40998</v>
       </c>
@@ -19126,15 +19653,19 @@
         <v>30.704999999999998</v>
       </c>
       <c r="C142">
-        <f>AVERAGE(B135:B149)</f>
+        <f t="shared" si="10"/>
         <v>26.076333333333331</v>
       </c>
       <c r="D142">
-        <f>(C143-C141)/(A143-A141)</f>
+        <f t="shared" si="11"/>
         <v>7.6666666666666593E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="E142">
+        <f t="shared" si="12"/>
+        <v>0.21399999999999864</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" s="1">
         <v>41029</v>
       </c>
@@ -19142,15 +19673,19 @@
         <v>29.824999999999999</v>
       </c>
       <c r="C143">
-        <f>AVERAGE(B136:B150)</f>
+        <f t="shared" si="10"/>
         <v>26.33</v>
       </c>
       <c r="D143">
-        <f>(C144-C142)/(A144-A142)</f>
+        <f t="shared" si="11"/>
         <v>1.3010752688172072E-2</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="E143">
+        <f t="shared" si="12"/>
+        <v>0.2536666666666676</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="1">
         <v>41060</v>
       </c>
@@ -19158,15 +19693,19 @@
         <v>27.07</v>
       </c>
       <c r="C144">
-        <f>AVERAGE(B137:B151)</f>
+        <f t="shared" si="10"/>
         <v>26.882999999999999</v>
       </c>
       <c r="D144">
-        <f>(C145-C143)/(A145-A143)</f>
+        <f t="shared" si="11"/>
         <v>2.3922222222222268E-2</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144">
+        <f t="shared" si="12"/>
+        <v>0.55300000000000082</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="1">
         <v>41089</v>
       </c>
@@ -19174,15 +19713,19 @@
         <v>27.94</v>
       </c>
       <c r="C145">
-        <f>AVERAGE(B138:B152)</f>
+        <f t="shared" si="10"/>
         <v>27.765333333333334</v>
       </c>
       <c r="D145">
-        <f>(C146-C144)/(A146-A144)</f>
+        <f t="shared" si="11"/>
         <v>3.3027322404371645E-2</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145">
+        <f t="shared" si="12"/>
+        <v>0.88233333333333519</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="1">
         <v>41121</v>
       </c>
@@ -19190,15 +19733,19 @@
         <v>29.26</v>
       </c>
       <c r="C146">
-        <f>AVERAGE(B139:B153)</f>
+        <f t="shared" si="10"/>
         <v>28.897666666666669</v>
       </c>
       <c r="D146">
-        <f>(C147-C145)/(A147-A145)</f>
+        <f t="shared" si="11"/>
         <v>3.4428571428571378E-2</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="E146">
+        <f t="shared" si="12"/>
+        <v>1.1323333333333352</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="1">
         <v>41152</v>
       </c>
@@ -19206,15 +19753,19 @@
         <v>30.32</v>
       </c>
       <c r="C147">
-        <f>AVERAGE(B140:B154)</f>
+        <f t="shared" si="10"/>
         <v>29.934333333333331</v>
       </c>
       <c r="D147">
-        <f>(C148-C146)/(A148-A146)</f>
+        <f t="shared" si="11"/>
         <v>3.3870056497175109E-2</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="E147">
+        <f t="shared" si="12"/>
+        <v>1.0366666666666617</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="1">
         <v>41180</v>
       </c>
@@ -19222,15 +19773,19 @@
         <v>24.664999999999999</v>
       </c>
       <c r="C148">
-        <f>AVERAGE(B141:B155)</f>
+        <f t="shared" si="10"/>
         <v>30.896000000000001</v>
       </c>
       <c r="D148">
-        <f>(C149-C147)/(A149-A147)</f>
+        <f t="shared" si="11"/>
         <v>3.4546448087431687E-2</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="E148">
+        <f t="shared" si="12"/>
+        <v>0.96166666666666956</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="1">
         <v>41213</v>
       </c>
@@ -19238,15 +19793,19 @@
         <v>27.41</v>
       </c>
       <c r="C149">
-        <f>AVERAGE(B142:B156)</f>
+        <f t="shared" si="10"/>
         <v>32.041666666666664</v>
       </c>
       <c r="D149">
-        <f>(C150-C148)/(A150-A148)</f>
+        <f t="shared" si="11"/>
         <v>2.9148148148148187E-2</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="E149">
+        <f t="shared" si="12"/>
+        <v>1.1456666666666635</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" s="1">
         <v>41243</v>
       </c>
@@ -19254,15 +19813,19 @@
         <v>25.89</v>
       </c>
       <c r="C150">
-        <f>AVERAGE(B143:B157)</f>
+        <f t="shared" si="10"/>
         <v>32.732333333333337</v>
       </c>
       <c r="D150">
-        <f>(C151-C149)/(A151-A149)</f>
+        <f t="shared" si="11"/>
         <v>2.7781420765027379E-2</v>
       </c>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="E150">
+        <f t="shared" si="12"/>
+        <v>0.69066666666667231</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151" s="1">
         <v>41274</v>
       </c>
@@ -19270,15 +19833,19 @@
         <v>29.5</v>
       </c>
       <c r="C151">
-        <f>AVERAGE(B144:B158)</f>
+        <f t="shared" si="10"/>
         <v>33.736333333333334</v>
       </c>
       <c r="D151">
-        <f>(C152-C150)/(A152-A150)</f>
+        <f t="shared" si="11"/>
         <v>3.3973118279569753E-2</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="E151">
+        <f t="shared" si="12"/>
+        <v>1.0039999999999978</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" s="1">
         <v>41305</v>
       </c>
@@ -19286,15 +19853,19 @@
         <v>34.604999999999997</v>
       </c>
       <c r="C152">
-        <f>AVERAGE(B145:B159)</f>
+        <f t="shared" si="10"/>
         <v>34.838666666666661</v>
       </c>
       <c r="D152">
-        <f>(C153-C151)/(A153-A151)</f>
+        <f t="shared" si="11"/>
         <v>4.0327683615819239E-2</v>
       </c>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="E152">
+        <f t="shared" si="12"/>
+        <v>1.1023333333333269</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153" s="1">
         <v>41333</v>
       </c>
@@ -19302,15 +19873,19 @@
         <v>39.18</v>
       </c>
       <c r="C153">
-        <f>AVERAGE(B146:B160)</f>
+        <f t="shared" si="10"/>
         <v>36.115666666666669</v>
       </c>
       <c r="D153">
-        <f>(C154-C152)/(A154-A152)</f>
+        <f t="shared" si="11"/>
         <v>4.7374269005848076E-2</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="E153">
+        <f t="shared" si="12"/>
+        <v>1.2770000000000081</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154" s="1">
         <v>41362</v>
       </c>
@@ -19318,15 +19893,19 @@
         <v>39.700000000000003</v>
       </c>
       <c r="C154">
-        <f>AVERAGE(B147:B161)</f>
+        <f t="shared" si="10"/>
         <v>37.539000000000001</v>
       </c>
       <c r="D154">
-        <f>(C155-C153)/(A155-A153)</f>
+        <f t="shared" si="11"/>
         <v>4.7311475409835997E-2</v>
       </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="E154">
+        <f t="shared" si="12"/>
+        <v>1.423333333333332</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155" s="1">
         <v>41394</v>
       </c>
@@ -19334,15 +19913,19 @@
         <v>40.104999999999997</v>
       </c>
       <c r="C155">
-        <f>AVERAGE(B148:B162)</f>
+        <f t="shared" si="10"/>
         <v>39.001666666666665</v>
       </c>
       <c r="D155">
-        <f>(C156-C154)/(A156-A154)</f>
+        <f t="shared" si="11"/>
         <v>5.6174603174603197E-2</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="E155">
+        <f t="shared" si="12"/>
+        <v>1.4626666666666637</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156" s="1">
         <v>41425</v>
       </c>
@@ -19350,15 +19933,19 @@
         <v>44.45</v>
       </c>
       <c r="C156">
-        <f>AVERAGE(B149:B163)</f>
+        <f t="shared" si="10"/>
         <v>41.078000000000003</v>
       </c>
       <c r="D156">
-        <f>(C157-C155)/(A157-A155)</f>
+        <f t="shared" si="11"/>
         <v>6.3666666666666732E-2</v>
       </c>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="E156">
+        <f t="shared" si="12"/>
+        <v>2.0763333333333378</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157" s="1">
         <v>41453</v>
       </c>
@@ -19366,15 +19953,19 @@
         <v>41.064999999999998</v>
       </c>
       <c r="C157">
-        <f>AVERAGE(B150:B164)</f>
+        <f t="shared" si="10"/>
         <v>42.758000000000003</v>
       </c>
       <c r="D157">
-        <f>(C158-C156)/(A158-A156)</f>
+        <f t="shared" si="11"/>
         <v>4.7292740046838533E-2</v>
       </c>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="E157">
+        <f t="shared" si="12"/>
+        <v>1.6799999999999997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158" s="1">
         <v>41486</v>
       </c>
@@ -19382,15 +19973,19 @@
         <v>44.884999999999998</v>
       </c>
       <c r="C158">
-        <f>AVERAGE(B151:B165)</f>
+        <f t="shared" si="10"/>
         <v>43.962857142857153</v>
       </c>
       <c r="D158">
-        <f>(C159-C157)/(A159-A157)</f>
+        <f t="shared" si="11"/>
         <v>3.6783882783882949E-2</v>
       </c>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="E158">
+        <f t="shared" si="12"/>
+        <v>1.2048571428571506</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
       <c r="A159" s="1">
         <v>41516</v>
       </c>
@@ -19398,15 +19993,19 @@
         <v>43.604999999999997</v>
       </c>
       <c r="C159">
-        <f>AVERAGE(B152:B166)</f>
+        <f t="shared" si="10"/>
         <v>45.075384615384628</v>
       </c>
       <c r="D159">
-        <f>(C160-C158)/(A160-A158)</f>
+        <f t="shared" si="11"/>
         <v>3.2541959406713297E-2</v>
       </c>
-    </row>
-    <row r="160" spans="1:4">
+      <c r="E159">
+        <f t="shared" si="12"/>
+        <v>1.112527472527475</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
       <c r="A160" s="1">
         <v>41547</v>
       </c>
@@ -19414,15 +20013,19 @@
         <v>47.094999999999999</v>
       </c>
       <c r="C160">
-        <f>AVERAGE(B153:B167)</f>
+        <f t="shared" si="10"/>
         <v>45.947916666666664</v>
       </c>
       <c r="D160">
-        <f>(C161-C159)/(A161-A159)</f>
+        <f t="shared" si="11"/>
         <v>2.3996729077373907E-2</v>
       </c>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="E160">
+        <f t="shared" si="12"/>
+        <v>0.87253205128203604</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161" s="1">
         <v>41578</v>
       </c>
@@ -19430,15 +20033,19 @@
         <v>50.61</v>
       </c>
       <c r="C161">
-        <f>AVERAGE(B154:B168)</f>
+        <f t="shared" si="10"/>
         <v>46.56318181818181</v>
       </c>
       <c r="D161">
-        <f>(C162-C160)/(A162-A160)</f>
+        <f t="shared" si="11"/>
         <v>2.1693055555555556E-2</v>
       </c>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="E161">
+        <f t="shared" si="12"/>
+        <v>0.61526515151514616</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162" s="1">
         <v>41607</v>
       </c>
@@ -19446,15 +20053,19 @@
         <v>52.26</v>
       </c>
       <c r="C162">
-        <f>AVERAGE(B155:B169)</f>
+        <f t="shared" si="10"/>
         <v>47.249499999999998</v>
       </c>
       <c r="D162">
-        <f>(C163-C161)/(A163-A161)</f>
+        <f t="shared" si="11"/>
         <v>2.4264778936910147E-2</v>
       </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="E162">
+        <f t="shared" si="12"/>
+        <v>0.68631818181818716</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163" s="1">
         <v>41639</v>
       </c>
@@ -19462,15 +20073,19 @@
         <v>55.81</v>
       </c>
       <c r="C163">
-        <f>AVERAGE(B156:B170)</f>
+        <f t="shared" si="10"/>
         <v>48.043333333333329</v>
       </c>
       <c r="D163">
-        <f>(C164-C162)/(A164-A162)</f>
+        <f t="shared" si="11"/>
         <v>1.9730158730158764E-2</v>
       </c>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="E163">
+        <f t="shared" si="12"/>
+        <v>0.79383333333333184</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164" s="1">
         <v>41670</v>
       </c>
@@ -19478,12 +20093,16 @@
         <v>52.61</v>
       </c>
       <c r="C164">
-        <f>AVERAGE(B157:B171)</f>
+        <f t="shared" si="10"/>
         <v>48.4925</v>
       </c>
       <c r="D164">
-        <f>(C165-C163)/(A165-A163)</f>
+        <f t="shared" si="11"/>
         <v>1.1538061272685061E-3</v>
+      </c>
+      <c r="E164">
+        <f t="shared" si="12"/>
+        <v>0.44916666666667027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>